<commit_message>
Added kernel SVR parameters to pred_par.xlsx of Magedburg dataset PCA embedding sequences
</commit_message>
<xml_diff>
--- a/Time_series_forecasting/a. Input time series sequences/2020-11-10_KS81_Nav_Pur_1_3_cpts/pred_par.xlsx
+++ b/Time_series_forecasting/a. Input time series sequences/2020-11-10_KS81_Nav_Pur_1_3_cpts/pred_par.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C681C9-C0B2-40F1-AFB0-5DBD3DA939C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BF076E-F8E9-4CFE-AB06-42F53B818B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Remarks :</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>tmax_pred</t>
+  </si>
+  <si>
+    <t>svr_kernel_scale</t>
+  </si>
+  <si>
+    <t>svr_epsilon</t>
+  </si>
+  <si>
+    <t>svr_box_constraint</t>
   </si>
 </sst>
 </file>
@@ -446,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -465,7 +474,7 @@
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -496,8 +505,17 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>170</v>
       </c>
@@ -528,66 +546,75 @@
       <c r="J2">
         <v>498</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>